<commit_message>
Update median of clusters (only mundist-f)-6.xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/median of clusters (only mundist-f)-6.xlsx
+++ b/migforecasting/clustering/median of clusters (only mundist-f)-6.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>clust</t>
   </si>
@@ -92,9 +92,6 @@
   <si>
     <t>5</t>
   </si>
-  <si>
-    <t>Mig prop</t>
-  </si>
 </sst>
 </file>
 
@@ -104,7 +101,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +114,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,22 +146,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -179,19 +158,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -295,32 +265,32 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>28076.460447825699</c:v>
+                  <c:v>27767</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>123856.99357367201</c:v>
+                  <c:v>25793.999999999902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71495.588441255299</c:v>
+                  <c:v>11739</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62240.295063542799</c:v>
+                  <c:v>20632.999999999902</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47731.931500533101</c:v>
+                  <c:v>29767</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72396.880334860602</c:v>
+                  <c:v>50487.499999999898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DE28-4E88-BB47-E153198D7264}"/>
+              <c16:uniqueId val="{00000000-0191-49B5-A15C-1E692B4E673F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -332,11 +302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1903152639"/>
-        <c:axId val="1903150559"/>
+        <c:axId val="1046193312"/>
+        <c:axId val="1046192480"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="1903152639"/>
+        <c:axId val="1046193312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +348,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903150559"/>
+        <c:crossAx val="1046192480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -386,7 +356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1903150559"/>
+        <c:axId val="1046192480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +376,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -437,7 +407,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903152639"/>
+        <c:crossAx val="1046193312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1036,15 +1006,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1351,30 +1321,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1429,755 +1388,704 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4">
-        <v>-217.487437185929</v>
-      </c>
-      <c r="C2" s="4">
-        <v>28076.460447825699</v>
+      <c r="B2" s="2">
+        <v>-125</v>
+      </c>
+      <c r="C2" s="2">
+        <v>27767</v>
       </c>
       <c r="D2" s="3">
-        <f>X2/C2</f>
-        <v>0.23482195554147511</v>
-      </c>
-      <c r="E2" s="3">
-        <v>28832.659355600001</v>
+        <f>Y2/C2</f>
+        <v>0.15143875823819605</v>
+      </c>
+      <c r="E2" s="4">
+        <v>19010.211839999902</v>
       </c>
       <c r="F2" s="3">
-        <f>Z2/C2</f>
-        <v>0.84554308897549324</v>
-      </c>
-      <c r="G2" s="7">
         <f>AA2/C2</f>
-        <v>2.4289202610942865E-2</v>
+        <v>0.47999783916159472</v>
+      </c>
+      <c r="G2" s="3">
+        <f>AB2/C2</f>
+        <v>1.7214679295566644E-2</v>
       </c>
       <c r="H2" s="3">
-        <f>AB2/C2</f>
-        <v>45.703825976871094</v>
-      </c>
-      <c r="I2" s="3">
-        <v>23.3300925925925</v>
-      </c>
-      <c r="J2" s="8">
-        <f>AD2/C2</f>
-        <v>2.7016070149210743E-3</v>
-      </c>
-      <c r="K2" s="8">
+        <f>AC2/C2</f>
+        <v>18.560126991032522</v>
+      </c>
+      <c r="I2" s="2">
+        <v>27.939999999999898</v>
+      </c>
+      <c r="J2" s="5">
         <f>AE2/C2</f>
-        <v>2.5567631892619166E-3</v>
-      </c>
-      <c r="L2" s="3">
-        <v>212.26793462109899</v>
-      </c>
-      <c r="M2" s="3">
-        <f>AG2/C2</f>
-        <v>0.16613383888716055</v>
-      </c>
-      <c r="N2" s="3">
-        <f>AH2/C2</f>
-        <v>0.24319526344363859</v>
-      </c>
-      <c r="O2" s="3">
-        <f>AI2/C2</f>
-        <v>3.2320631173605103</v>
-      </c>
-      <c r="P2" s="8">
-        <f>AJ2/C2</f>
-        <v>6.1572420618916611E-4</v>
+        <v>3.4213274750603236E-3</v>
+      </c>
+      <c r="K2" s="5">
+        <f>AF2/C2</f>
+        <v>2.1248244318795694E-3</v>
+      </c>
+      <c r="L2" s="2">
+        <v>430.4</v>
+      </c>
+      <c r="M2" s="2">
+        <v>250298.99999999901</v>
+      </c>
+      <c r="N2" s="2">
+        <v>22711.08</v>
+      </c>
+      <c r="O2" s="2">
+        <v>3473352.9905999899</v>
+      </c>
+      <c r="P2" s="5">
+        <f>AK2/C2</f>
+        <v>1.0444052292289409E-3</v>
       </c>
       <c r="Q2" s="3">
-        <f>AK2/C2</f>
-        <v>6.1985571705407236E-2</v>
-      </c>
-      <c r="R2" s="3">
         <f>AL2/C2</f>
-        <v>100.41643548564809</v>
-      </c>
-      <c r="S2" s="6">
-        <f>B2/C2</f>
-        <v>-7.7462555363801812E-3</v>
-      </c>
-      <c r="X2" s="4">
-        <v>6592.9693470413104</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>28832.659355600001</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>23739.857094552801</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>681.95483641536202</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>1283201.6623539301</v>
-      </c>
-      <c r="AC2" s="4">
-        <v>23.3300925925925</v>
-      </c>
-      <c r="AD2" s="4">
-        <v>75.8515625</v>
-      </c>
-      <c r="AE2" s="4">
-        <v>71.784860557768894</v>
-      </c>
-      <c r="AF2" s="4">
-        <v>212.26793462109899</v>
-      </c>
-      <c r="AG2" s="4">
-        <v>4664.4501565608098</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>6828.0621951738704</v>
-      </c>
-      <c r="AI2" s="4">
-        <v>90744.892279448599</v>
-      </c>
-      <c r="AJ2" s="4">
-        <v>17.287356321838999</v>
-      </c>
-      <c r="AK2" s="4">
-        <v>1740.3354523227299</v>
-      </c>
-      <c r="AL2" s="4">
-        <v>2819338.0792244398</v>
+        <v>4.3829005654193468E-2</v>
+      </c>
+      <c r="R2" s="2">
+        <v>2228908.4339600001</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>4204.99999999999</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>19010.211839999902</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>13328.1</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>477.99999999999898</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>515359.04616000003</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>27.939999999999898</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>95</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>430.4</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>250298.99999999901</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>22711.08</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>3473352.9905999899</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>29</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>1216.99999999999</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>2228908.4339600001</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="4">
-        <v>-456.72361809045202</v>
-      </c>
-      <c r="C3" s="4">
-        <v>123856.99357367201</v>
+      <c r="B3" s="2">
+        <v>-96.499999999999901</v>
+      </c>
+      <c r="C3" s="2">
+        <v>25793.999999999902</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D7" si="0">X3/C3</f>
-        <v>0.25248185617910673</v>
-      </c>
-      <c r="E3" s="3">
-        <v>33489.866736178403</v>
+        <f t="shared" ref="D3:D7" si="0">Y3/C3</f>
+        <v>0.13867566100643575</v>
+      </c>
+      <c r="E3" s="4">
+        <v>19000.57358</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F7" si="1">Z3/C3</f>
-        <v>1.0448250067736842</v>
-      </c>
-      <c r="G3" s="7">
-        <f t="shared" ref="G3:G7" si="2">AA3/C3</f>
-        <v>3.4720806047465046E-2</v>
+        <f t="shared" ref="F3:F7" si="1">AA3/C3</f>
+        <v>0.45362875087229371</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G7" si="2">AB3/C3</f>
+        <v>1.9810808715205162E-2</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H7" si="3">AB3/C3</f>
-        <v>62.592103790502748</v>
-      </c>
-      <c r="I3" s="3">
-        <v>19.826851851851799</v>
-      </c>
-      <c r="J3" s="8">
-        <f t="shared" ref="J3:J7" si="4">AD3/C3</f>
-        <v>2.0789790412346592E-3</v>
-      </c>
-      <c r="K3" s="8">
-        <f t="shared" ref="K3:K7" si="5">AE3/C3</f>
-        <v>3.4636719947898974E-3</v>
-      </c>
-      <c r="L3" s="3">
-        <v>444.73245170876601</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" ref="M3:M7" si="6">AG3/C3</f>
-        <v>8.9945595556999589E-2</v>
-      </c>
-      <c r="N3" s="3">
-        <f t="shared" ref="N3:N7" si="7">AH3/C3</f>
-        <v>0.21909772176143472</v>
-      </c>
-      <c r="O3" s="3">
-        <f t="shared" ref="O3:O7" si="8">AI3/C3</f>
-        <v>2.5055970848449074</v>
-      </c>
-      <c r="P3" s="8">
-        <f t="shared" ref="P3:P7" si="9">AJ3/C3</f>
-        <v>3.3149094031534196E-4</v>
+        <f t="shared" ref="H3:H7" si="3">AC3/C3</f>
+        <v>20.382080135496665</v>
+      </c>
+      <c r="I3" s="2">
+        <v>30.434999999999999</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J7" si="4">AE3/C3</f>
+        <v>3.4504148251531495E-3</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K7" si="5">AF3/C3</f>
+        <v>1.7833604714274666E-3</v>
+      </c>
+      <c r="L3" s="2">
+        <v>436.3</v>
+      </c>
+      <c r="M3" s="2">
+        <v>61787.499999999898</v>
+      </c>
+      <c r="N3" s="2">
+        <v>77442.764999999999</v>
+      </c>
+      <c r="O3" s="2">
+        <v>2924436.5</v>
+      </c>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:P7" si="6">AK3/C3</f>
+        <v>1.1630611770179155E-3</v>
       </c>
       <c r="Q3" s="3">
-        <f t="shared" ref="Q3:Q7" si="10">AK3/C3</f>
-        <v>6.3102052914745785E-2</v>
-      </c>
-      <c r="R3" s="3">
-        <f>AL3/C3</f>
-        <v>323.28952580241673</v>
-      </c>
-      <c r="S3" s="6">
-        <f t="shared" ref="S3:S7" si="11">B3/C3</f>
-        <v>-3.6875077047529492E-3</v>
-      </c>
-      <c r="X3" s="4">
-        <v>31271.643638244401</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>33489.866736178403</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>129408.88414958</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>4300.4146514935901</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>7752469.7969429102</v>
-      </c>
-      <c r="AC3" s="4">
-        <v>19.826851851851799</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>257.49609375</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>429</v>
-      </c>
-      <c r="AF3" s="4">
-        <v>444.73245170876601</v>
-      </c>
-      <c r="AG3" s="4">
-        <v>11140.3910508834</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>27136.785116212199</v>
-      </c>
-      <c r="AI3" s="4">
-        <v>310335.72203584702</v>
-      </c>
-      <c r="AJ3" s="4">
-        <v>41.057471264367798</v>
-      </c>
-      <c r="AK3" s="4">
-        <v>7815.6305623471799</v>
-      </c>
-      <c r="AL3" s="4">
-        <v>40041668.719745398</v>
+        <f t="shared" ref="Q3:Q7" si="7">AL3/C3</f>
+        <v>4.2064045902147948E-2</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1966599.34497499</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>3576.99999999999</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>19000.57358</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>11700.8999999999</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>511</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>525735.37501499895</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>30.434999999999999</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>89</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>45.999999999999901</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>436.3</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>61787.499999999898</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>77442.764999999999</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>2924436.5</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>30</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>1085</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>1966599.34497499</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4">
-        <v>-436.33417085427101</v>
-      </c>
-      <c r="C4" s="4">
-        <v>71495.588441255299</v>
+      <c r="B4" s="2">
+        <v>-81.999999999999901</v>
+      </c>
+      <c r="C4" s="2">
+        <v>11739</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>0.29513633181407961</v>
-      </c>
-      <c r="E4" s="3">
-        <v>34679.537979299799</v>
+        <v>0.15009796405145243</v>
+      </c>
+      <c r="E4" s="4">
+        <v>18107.031070000001</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>1.0023558458825217</v>
-      </c>
-      <c r="G4" s="7">
+        <v>0.51145753471334776</v>
+      </c>
+      <c r="G4" s="3">
         <f t="shared" si="2"/>
-        <v>3.278505559865709E-2</v>
+        <v>1.5844620495783203E-2</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="3"/>
-        <v>54.050511196953096</v>
-      </c>
-      <c r="I4" s="3">
-        <v>20.870370370370299</v>
-      </c>
-      <c r="J4" s="8">
+        <v>20.003460076667434</v>
+      </c>
+      <c r="I4" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="J4" s="5">
         <f t="shared" si="4"/>
-        <v>2.0939338288404677E-3</v>
-      </c>
-      <c r="K4" s="8">
+        <v>3.4074452679103842E-3</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="5"/>
-        <v>3.25119661516504E-3</v>
-      </c>
-      <c r="L4" s="3">
-        <v>340.04374442793397</v>
-      </c>
-      <c r="M4" s="3">
+        <v>1.8740948973507028E-3</v>
+      </c>
+      <c r="L4" s="2">
+        <v>286.39999999999998</v>
+      </c>
+      <c r="M4" s="2">
+        <v>22423.999999999902</v>
+      </c>
+      <c r="N4" s="2">
+        <v>8878.1699999999892</v>
+      </c>
+      <c r="O4" s="2">
+        <v>657408.45539999905</v>
+      </c>
+      <c r="P4" s="5">
         <f t="shared" si="6"/>
-        <v>8.7511392451058309E-2</v>
-      </c>
-      <c r="N4" s="3">
+        <v>1.4481642388619134E-3</v>
+      </c>
+      <c r="Q4" s="3">
         <f t="shared" si="7"/>
-        <v>0.20123791865859891</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" si="8"/>
-        <v>2.3383132819865877</v>
-      </c>
-      <c r="P4" s="8">
-        <f t="shared" si="9"/>
-        <v>3.9291870499213235E-4</v>
-      </c>
-      <c r="Q4" s="3">
-        <f t="shared" si="10"/>
-        <v>6.9760744139070963E-2</v>
-      </c>
-      <c r="R4" s="3">
-        <f>AL4/C4</f>
-        <v>481.58099208206573</v>
-      </c>
-      <c r="S4" s="6">
-        <f t="shared" si="11"/>
-        <v>-6.1029523690512332E-3</v>
-      </c>
-      <c r="X4" s="4">
-        <v>21100.9457134412</v>
-      </c>
-      <c r="Y4" s="4">
-        <v>34679.537979299799</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>71664.021028903095</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>2343.9868421052602</v>
-      </c>
-      <c r="AB4" s="4">
-        <v>3864373.1035768199</v>
-      </c>
-      <c r="AC4" s="4">
-        <v>20.870370370370299</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>149.70703125</v>
-      </c>
-      <c r="AE4" s="4">
-        <v>232.44621513944199</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>340.04374442793397</v>
-      </c>
-      <c r="AG4" s="4">
-        <v>6256.6784986020402</v>
-      </c>
-      <c r="AH4" s="4">
-        <v>14387.623411189999</v>
-      </c>
-      <c r="AI4" s="4">
-        <v>167179.08405563401</v>
-      </c>
-      <c r="AJ4" s="4">
-        <v>28.091954022988499</v>
-      </c>
-      <c r="AK4" s="4">
-        <v>4987.5854523227299</v>
-      </c>
-      <c r="AL4" s="4">
-        <v>34430916.411030799</v>
+        <v>4.7619047619047533E-2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>386760.31725999998</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>1762</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>18107.031070000001</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>6003.99999999999</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>185.99999999999901</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>234820.617839999</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>21.999999999999901</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>286.39999999999998</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>22423.999999999902</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>8878.1699999999892</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>657408.45539999905</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>17</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>558.99999999999898</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>386760.31725999998</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4">
-        <v>-250.11055276381799</v>
-      </c>
-      <c r="C5" s="4">
-        <v>62240.295063542799</v>
+      <c r="B5" s="2">
+        <v>-134.99999999999901</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20632.999999999902</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>0.2196016437164878</v>
-      </c>
-      <c r="E5" s="3">
-        <v>30154.966507012501</v>
+        <v>0.15387970726506106</v>
+      </c>
+      <c r="E5" s="4">
+        <v>18637.383989999998</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>0.75216931040746926</v>
-      </c>
-      <c r="G5" s="7">
+        <v>0.51732661270779579</v>
+      </c>
+      <c r="G5" s="3">
         <f t="shared" si="2"/>
-        <v>3.0834727178295111E-2</v>
+        <v>1.7980904376484308E-2</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="3"/>
-        <v>46.767000685184634</v>
-      </c>
-      <c r="I5" s="3">
-        <v>22.584722222222201</v>
-      </c>
-      <c r="J5" s="8">
+        <v>19.145869483352005</v>
+      </c>
+      <c r="I5" s="2">
+        <v>27.799999999999901</v>
+      </c>
+      <c r="J5" s="5">
         <f t="shared" si="4"/>
-        <v>2.8542979040929984E-3</v>
-      </c>
-      <c r="K5" s="8">
+        <v>3.5380216158581081E-3</v>
+      </c>
+      <c r="K5" s="5">
         <f t="shared" si="5"/>
-        <v>2.4714648450521516E-3</v>
-      </c>
-      <c r="L5" s="3">
-        <v>323.36766716196098</v>
-      </c>
-      <c r="M5" s="3">
+        <v>2.0840401298890181E-3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>387.99999999999898</v>
+      </c>
+      <c r="M5" s="2">
+        <v>55202.26</v>
+      </c>
+      <c r="N5" s="2">
+        <v>17287.07</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1653334.55999999</v>
+      </c>
+      <c r="P5" s="5">
         <f t="shared" si="6"/>
-        <v>0.2094156418187903</v>
-      </c>
-      <c r="N5" s="3">
+        <v>1.308583337372177E-3</v>
+      </c>
+      <c r="Q5" s="3">
         <f t="shared" si="7"/>
-        <v>1.0256367322483171</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="8"/>
-        <v>7.2237224347371667</v>
-      </c>
-      <c r="P5" s="8">
-        <f t="shared" si="9"/>
-        <v>5.2078469535461042E-4</v>
-      </c>
-      <c r="Q5" s="3">
-        <f t="shared" si="10"/>
-        <v>5.515773956124715E-2</v>
-      </c>
-      <c r="R5" s="3">
-        <f>AL5/C5</f>
-        <v>253.58532097969939</v>
-      </c>
-      <c r="S5" s="6">
-        <f t="shared" si="11"/>
-        <v>-4.0184666944215698E-3</v>
-      </c>
-      <c r="X5" s="4">
-        <v>13668.0711013532</v>
-      </c>
-      <c r="Y5" s="4">
-        <v>30154.966507012501</v>
-      </c>
-      <c r="Z5" s="4">
-        <v>46815.239817502399</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>1919.1625177809301</v>
-      </c>
-      <c r="AB5" s="4">
-        <v>2910791.9218827998</v>
-      </c>
-      <c r="AC5" s="4">
-        <v>22.584722222222201</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>177.65234375</v>
-      </c>
-      <c r="AE5" s="4">
-        <v>153.82470119521901</v>
-      </c>
-      <c r="AF5" s="4">
-        <v>323.36766716196098</v>
-      </c>
-      <c r="AG5" s="4">
-        <v>13034.091337722701</v>
-      </c>
-      <c r="AH5" s="4">
-        <v>63835.932843143099</v>
-      </c>
-      <c r="AI5" s="4">
-        <v>449606.61579517502</v>
-      </c>
-      <c r="AJ5" s="4">
-        <v>32.413793103448199</v>
-      </c>
-      <c r="AK5" s="4">
-        <v>3433.0339853300702</v>
-      </c>
-      <c r="AL5" s="4">
-        <v>15783225.2015597</v>
+        <v>5.0598555711724176E-2</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1013598.8844</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>3174.99999999999</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>18637.383989999998</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>10673.9999999999</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>370.99999999999898</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>395036.72505000001</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>27.799999999999901</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>42.999999999999901</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>387.99999999999898</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>55202.26</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>17287.07</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>1653334.55999999</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>27</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>1044</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>1013598.8844</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4">
-        <v>-356.135678391959</v>
-      </c>
-      <c r="C6" s="4">
-        <v>47731.931500533101</v>
+      <c r="B6" s="2">
+        <v>-163.99999999999901</v>
+      </c>
+      <c r="C6" s="2">
+        <v>29767</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>0.24021551407897962</v>
-      </c>
-      <c r="E6" s="3">
-        <v>29328.3996026799</v>
+        <v>0.18947156246850505</v>
+      </c>
+      <c r="E6" s="4">
+        <v>22219.616679999999</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>0.83875677625560696</v>
-      </c>
-      <c r="G6" s="7">
+        <v>0.6014378338428461</v>
+      </c>
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
-        <v>2.7481357308277159E-2</v>
+        <v>2.11307824100514E-2</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="3"/>
-        <v>42.323187815804758</v>
-      </c>
-      <c r="I6" s="3">
-        <v>20.870370370370299</v>
-      </c>
-      <c r="J6" s="8">
+        <v>23.460937424328954</v>
+      </c>
+      <c r="I6" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="J6" s="5">
         <f t="shared" si="4"/>
-        <v>2.9691372587429686E-3</v>
-      </c>
-      <c r="K6" s="8">
+        <v>2.5531628985117748E-3</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="5"/>
-        <v>2.8646037030275189E-3</v>
-      </c>
-      <c r="L6" s="3">
-        <v>277.37875185735498</v>
-      </c>
-      <c r="M6" s="3">
+        <v>2.250814660530114E-3</v>
+      </c>
+      <c r="L6" s="2">
+        <v>454.5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>27778.999999999902</v>
+      </c>
+      <c r="N6" s="2">
+        <v>18681.559999999899</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1089390.87169999</v>
+      </c>
+      <c r="P6" s="5">
         <f t="shared" si="6"/>
-        <v>0.26163676668822888</v>
-      </c>
-      <c r="N6" s="3">
+        <v>8.3985621661571207E-4</v>
+      </c>
+      <c r="Q6" s="3">
         <f t="shared" si="7"/>
-        <v>0.2878637450845089</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" si="8"/>
-        <v>5.5068409437387693</v>
-      </c>
-      <c r="P6" s="8">
-        <f t="shared" si="9"/>
-        <v>5.8853587399191568E-4</v>
-      </c>
-      <c r="Q6" s="3">
-        <f t="shared" si="10"/>
-        <v>6.5968425491287563E-2</v>
-      </c>
-      <c r="R6" s="3">
-        <f>AL6/C6</f>
-        <v>155.88181046666003</v>
-      </c>
-      <c r="S6" s="6">
-        <f t="shared" si="11"/>
-        <v>-7.4611621025221127E-3</v>
-      </c>
-      <c r="X6" s="4">
-        <v>11465.9504633832</v>
-      </c>
-      <c r="Y6" s="4">
-        <v>29328.3996026799</v>
-      </c>
-      <c r="Z6" s="4">
-        <v>40035.480989840602</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>1311.73826458036</v>
-      </c>
-      <c r="AB6" s="4">
-        <v>2020167.50170819</v>
-      </c>
-      <c r="AC6" s="4">
-        <v>20.870370370370299</v>
-      </c>
-      <c r="AD6" s="4">
-        <v>141.72265625</v>
-      </c>
-      <c r="AE6" s="4">
-        <v>136.73306772908299</v>
-      </c>
-      <c r="AF6" s="4">
-        <v>277.37875185735498</v>
-      </c>
-      <c r="AG6" s="4">
-        <v>12488.428225583501</v>
-      </c>
-      <c r="AH6" s="4">
-        <v>13740.292561860701</v>
-      </c>
-      <c r="AI6" s="4">
-        <v>262852.15471087</v>
-      </c>
-      <c r="AJ6" s="4">
-        <v>28.091954022988499</v>
-      </c>
-      <c r="AK6" s="4">
-        <v>3148.8003667481598</v>
-      </c>
-      <c r="AL6" s="4">
-        <v>7440539.8993736999</v>
+        <v>5.2978130144118993E-2</v>
+      </c>
+      <c r="R6" s="2">
+        <v>5149712.4000000004</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>5639.99999999999</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>22219.616679999999</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>17903</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>629</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>698361.72430999996</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>66.999999999999901</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>454.5</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>27778.999999999902</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>18681.559999999899</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>1089390.87169999</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>24.999999999999901</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>1576.99999999999</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>5149712.4000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4">
-        <v>-377.88442211055201</v>
-      </c>
-      <c r="C7" s="4">
-        <v>72396.880334860602</v>
+      <c r="B7" s="2">
+        <v>-167.99999999999901</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50487.499999999898</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>0.23015171829700062</v>
-      </c>
-      <c r="E7" s="3">
-        <v>30145.1214815237</v>
+        <v>0.16053478583807906</v>
+      </c>
+      <c r="E7" s="4">
+        <v>21125.68202</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>0.77078522522792547</v>
-      </c>
-      <c r="G7" s="7">
+        <v>0.63497499381035039</v>
+      </c>
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>2.6817753524256308E-2</v>
+        <v>2.2718494676900267E-2</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="3"/>
-        <v>41.707690917257999</v>
-      </c>
-      <c r="I7" s="3">
-        <v>20.792106481481401</v>
-      </c>
-      <c r="J7" s="8">
+        <v>27.337661854023327</v>
+      </c>
+      <c r="I7" s="2">
+        <v>26.58</v>
+      </c>
+      <c r="J7" s="5">
         <f t="shared" si="4"/>
-        <v>2.9777267197547276E-3</v>
-      </c>
-      <c r="K7" s="8">
+        <v>2.545184451596935E-3</v>
+      </c>
+      <c r="K7" s="5">
         <f t="shared" si="5"/>
-        <v>3.021855463310472E-3</v>
-      </c>
-      <c r="L7" s="3">
-        <v>348.78942050519998</v>
-      </c>
-      <c r="M7" s="3">
+        <v>2.3570190641247686E-3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>600.04999999999995</v>
+      </c>
+      <c r="M7" s="2">
+        <v>53335.889999999898</v>
+      </c>
+      <c r="N7" s="2">
+        <v>34494.949999999997</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2131489.5078999898</v>
+      </c>
+      <c r="P7" s="5">
         <f t="shared" si="6"/>
-        <v>0.74975325291691397</v>
-      </c>
-      <c r="N7" s="3">
+        <v>7.7246843278039269E-4</v>
+      </c>
+      <c r="Q7" s="3">
         <f t="shared" si="7"/>
-        <v>0.27673108770900573</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="8"/>
-        <v>7.4564632157167576</v>
-      </c>
-      <c r="P7" s="8">
-        <f t="shared" si="9"/>
-        <v>4.6264773728703086E-4</v>
-      </c>
-      <c r="Q7" s="3">
-        <f t="shared" si="10"/>
-        <v>5.7552791273810661E-2</v>
-      </c>
-      <c r="R7" s="3">
-        <f>AL7/C7</f>
-        <v>243.47185998021556</v>
-      </c>
-      <c r="S7" s="6">
-        <f t="shared" si="11"/>
-        <v>-5.2196230053381566E-3</v>
-      </c>
-      <c r="X7" s="4">
-        <v>16662.266408410502</v>
-      </c>
-      <c r="Y7" s="4">
-        <v>30145.1214815237</v>
-      </c>
-      <c r="Z7" s="4">
-        <v>55802.4457147047</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>1941.52169274537</v>
-      </c>
-      <c r="AB7" s="4">
-        <v>3019506.7083800798</v>
-      </c>
-      <c r="AC7" s="4">
-        <v>20.792106481481401</v>
-      </c>
-      <c r="AD7" s="4">
-        <v>215.578125</v>
-      </c>
-      <c r="AE7" s="4">
-        <v>218.77290836653299</v>
-      </c>
-      <c r="AF7" s="4">
-        <v>348.78942050519998</v>
-      </c>
-      <c r="AG7" s="4">
-        <v>54279.796532098298</v>
-      </c>
-      <c r="AH7" s="4">
-        <v>20034.4674418047</v>
-      </c>
-      <c r="AI7" s="4">
-        <v>539824.67514953599</v>
-      </c>
-      <c r="AJ7" s="4">
-        <v>33.494252873563198</v>
-      </c>
-      <c r="AK7" s="4">
-        <v>4166.64254278728</v>
-      </c>
-      <c r="AL7" s="4">
-        <v>17626603.111893602</v>
+        <v>4.8516959643476208E-2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>4985951.7012949996</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>8105</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>21125.68202</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>32058.3</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1147</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>1380210.202855</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>26.58</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>128.5</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>118.99999999999901</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>600.04999999999995</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>53335.889999999898</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>34494.949999999997</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>2131489.5078999898</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>2449.5</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>4985951.7012949996</v>
       </c>
     </row>
   </sheetData>
@@ -2385,19 +2293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S7">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X7">
+  <conditionalFormatting sqref="Y2:Y7">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2409,7 +2305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y7">
+  <conditionalFormatting sqref="Z2:Z7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2421,7 +2317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z7">
+  <conditionalFormatting sqref="AA2:AA7">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2433,7 +2329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA7">
+  <conditionalFormatting sqref="AB2:AB7">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2445,7 +2341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB7">
+  <conditionalFormatting sqref="AC2:AC7">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2457,7 +2353,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC7">
+  <conditionalFormatting sqref="AD2:AD7">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2469,7 +2365,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD7">
+  <conditionalFormatting sqref="AE2:AE7">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2481,7 +2377,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE7">
+  <conditionalFormatting sqref="AF2:AF7">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2493,7 +2389,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF2:AF7">
+  <conditionalFormatting sqref="AG2:AG7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2505,7 +2401,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG7">
+  <conditionalFormatting sqref="AH2:AH7">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2517,7 +2413,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH7">
+  <conditionalFormatting sqref="AI2:AI7">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2529,7 +2425,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:AI7">
+  <conditionalFormatting sqref="AJ2:AJ7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2541,7 +2437,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AJ7">
+  <conditionalFormatting sqref="AK2:AK7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2553,7 +2449,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK7">
+  <conditionalFormatting sqref="AL2:AL7">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2565,7 +2461,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL2:AL7">
+  <conditionalFormatting sqref="AM2:AM7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>